<commit_message>
more config added to MOSTRO_HOME
</commit_message>
<xml_diff>
--- a/data/info_intersecciones.xlsx
+++ b/data/info_intersecciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ARS" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="144">
   <si>
     <t>Intersección</t>
   </si>
@@ -154,9 +154,6 @@
     <t>cr70_cll43</t>
   </si>
   <si>
-    <t>av33_cr74</t>
-  </si>
-  <si>
     <t>tv39b_cq74b</t>
   </si>
   <si>
@@ -196,12 +193,6 @@
     <t>cll44_cr80a</t>
   </si>
   <si>
-    <t>tv39b_cq2</t>
-  </si>
-  <si>
-    <t>Circular 72</t>
-  </si>
-  <si>
     <t>cll44_cr84</t>
   </si>
   <si>
@@ -211,18 +202,6 @@
     <t>Carrera 84 &gt;(S)</t>
   </si>
   <si>
-    <t>cr76_cll33a</t>
-  </si>
-  <si>
-    <t>Calle 33A &gt;Occidente</t>
-  </si>
-  <si>
-    <t>Calle 33A &gt;Oriente</t>
-  </si>
-  <si>
-    <t>cr76_cll32f</t>
-  </si>
-  <si>
     <t>Calle 32F &gt;Occidente</t>
   </si>
   <si>
@@ -241,22 +220,10 @@
     <t>Carrera 79</t>
   </si>
   <si>
-    <t>cr78_cll44a</t>
-  </si>
-  <si>
-    <t>Calle 44A</t>
-  </si>
-  <si>
     <t>cll44_cr74</t>
   </si>
   <si>
     <t>Carrera 74</t>
-  </si>
-  <si>
-    <t>cr73_cll43</t>
-  </si>
-  <si>
-    <t>cr70_cll44a</t>
   </si>
   <si>
     <t>cr66b_cll34a</t>
@@ -613,47 +580,47 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -945,7 +912,7 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -956,766 +923,766 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>152</v>
+        <v>74</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="18" t="s">
-        <v>151</v>
+      <c r="D3" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="12"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="7"/>
-      <c r="D4" s="18" t="s">
-        <v>150</v>
+      <c r="D4" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="18" t="s">
-        <v>149</v>
+      <c r="D5" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>148</v>
+        <v>86</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="9"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="18" t="s">
-        <v>147</v>
+      <c r="D7" s="6" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="9"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="18" t="s">
-        <v>146</v>
+      <c r="D8" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="10"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="18" t="s">
-        <v>145</v>
+      <c r="D9" s="6" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>144</v>
+        <v>74</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="12"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="18" t="s">
-        <v>143</v>
+      <c r="D11" s="6" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="12"/>
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="18" t="s">
-        <v>142</v>
+      <c r="D12" s="6" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="18" t="s">
-        <v>141</v>
+      <c r="D13" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="12"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>140</v>
+        <v>86</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="12"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="18" t="s">
-        <v>139</v>
+      <c r="D15" s="6" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="18" t="s">
-        <v>138</v>
+      <c r="D16" s="6" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="18" t="s">
-        <v>137</v>
+      <c r="D17" s="6" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>136</v>
+      <c r="C18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="18" t="s">
-        <v>135</v>
+      <c r="A19" s="11"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="6" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="18" t="s">
-        <v>134</v>
+      <c r="A20" s="11"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="6" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="12"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>133</v>
+        <v>86</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="9"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="18" t="s">
-        <v>132</v>
+      <c r="D22" s="6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="9"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="18" t="s">
-        <v>131</v>
+      <c r="D23" s="6" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>88</v>
+        <v>74</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="6" t="s">
-        <v>87</v>
+      <c r="D25" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="11"/>
+      <c r="B26" s="8" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="11"/>
+      <c r="B27" s="10"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="10"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="6" t="s">
-        <v>93</v>
+      <c r="D29" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="11"/>
+      <c r="B30" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>91</v>
+        <v>74</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="8"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="6" t="s">
-        <v>90</v>
+      <c r="D31" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>130</v>
+      <c r="C32" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="6" t="s">
-        <v>129</v>
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="6" t="s">
-        <v>128</v>
+      <c r="A34" s="11"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>127</v>
+        <v>86</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="16"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="6" t="s">
-        <v>126</v>
+      <c r="D36" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="15"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="6" t="s">
-        <v>125</v>
+      <c r="D37" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="11"/>
+      <c r="B38" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>124</v>
+      <c r="C38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="6" t="s">
-        <v>123</v>
+      <c r="A39" s="11"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="5" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="6" t="s">
-        <v>122</v>
+      <c r="A40" s="11"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>121</v>
+        <v>86</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="7"/>
-      <c r="D42" s="6" t="s">
-        <v>120</v>
+      <c r="D42" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="11"/>
+      <c r="A43" s="11"/>
+      <c r="B43" s="10"/>
       <c r="C43" s="7"/>
-      <c r="D43" s="6" t="s">
-        <v>119</v>
+      <c r="D43" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="17" t="s">
+      <c r="A44" s="11"/>
+      <c r="B44" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>118</v>
+      <c r="C44" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="6" t="s">
-        <v>117</v>
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="5" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="6" t="s">
-        <v>116</v>
+      <c r="A46" s="11"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="5" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="16"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>115</v>
+        <v>86</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="16"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="7"/>
-      <c r="D48" s="6" t="s">
-        <v>114</v>
+      <c r="D48" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="15"/>
       <c r="C49" s="7"/>
-      <c r="D49" s="6" t="s">
-        <v>113</v>
+      <c r="D49" s="5" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C50" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="11"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="11"/>
+      <c r="B62" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="10"/>
-      <c r="D63" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D65" s="6" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
-      <c r="B66" s="8"/>
+      <c r="A66" s="11"/>
+      <c r="B66" s="17"/>
       <c r="C66" s="7"/>
-      <c r="D66" s="6" t="s">
-        <v>95</v>
+      <c r="D66" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="A67" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>94</v>
+      <c r="C67" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="10"/>
-      <c r="D68" s="6" t="s">
-        <v>93</v>
+      <c r="A68" s="11"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="10"/>
-      <c r="D69" s="6" t="s">
-        <v>92</v>
+      <c r="A69" s="11"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="9" t="s">
+      <c r="A70" s="11"/>
+      <c r="B70" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>91</v>
+      <c r="C70" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="6" t="s">
-        <v>90</v>
+      <c r="A71" s="11"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="4"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="6" t="s">
-        <v>89</v>
+      <c r="A72" s="11"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="13" t="s">
+      <c r="A73" s="11"/>
+      <c r="B73" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>88</v>
+      <c r="C73" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="6" t="s">
-        <v>87</v>
+      <c r="A74" s="11"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="10"/>
-      <c r="D75" s="6" t="s">
-        <v>86</v>
+      <c r="A75" s="11"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="5" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="9" t="s">
+      <c r="A76" s="11"/>
+      <c r="B76" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>84</v>
+        <v>74</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="8"/>
+      <c r="A77" s="11"/>
+      <c r="B77" s="17"/>
       <c r="C77" s="7"/>
-      <c r="D77" s="6" t="s">
-        <v>83</v>
+      <c r="D77" s="5" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="C70:C72"/>
+    <mergeCell ref="C73:C75"/>
+    <mergeCell ref="C76:C77"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C24:C25"/>
     <mergeCell ref="B62:B66"/>
     <mergeCell ref="B58:B61"/>
     <mergeCell ref="B50:B57"/>
     <mergeCell ref="C50:C53"/>
     <mergeCell ref="C54:C57"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="C70:C72"/>
-    <mergeCell ref="C73:C75"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="A32:A49"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="C35:C37"/>
     <mergeCell ref="C38:C40"/>
     <mergeCell ref="C41:C43"/>
     <mergeCell ref="C44:C46"/>
     <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="A24:A31"/>
     <mergeCell ref="A50:A66"/>
     <mergeCell ref="A67:A77"/>
     <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A32:A49"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B67:B69"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="B10:B17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1723,10 +1690,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B115"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1744,7 +1711,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1752,19 +1719,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="11"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="11"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1772,25 +1739,25 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="11"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="11"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1798,25 +1765,25 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="11"/>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1824,19 +1791,19 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1844,19 +1811,19 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1864,19 +1831,19 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
+      <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1884,19 +1851,19 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
+      <c r="A23" s="11"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="11" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1904,19 +1871,19 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
+      <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
+      <c r="A27" s="11"/>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1924,19 +1891,19 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
+      <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1944,25 +1911,25 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="11"/>
       <c r="B32" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="11"/>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
+      <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1970,13 +1937,13 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="11" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1984,19 +1951,19 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
+      <c r="A39" s="11"/>
       <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="11" t="s">
         <v>35</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2004,25 +1971,25 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
+      <c r="A41" s="11"/>
       <c r="B41" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
+      <c r="A44" s="11" t="s">
         <v>36</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2030,13 +1997,13 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="11" t="s">
         <v>38</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2044,19 +2011,19 @@
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="11" t="s">
         <v>41</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2064,19 +2031,19 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
+      <c r="A52" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2084,53 +2051,53 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>12</v>
+      <c r="B54" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="3" t="s">
-        <v>15</v>
+      <c r="A55" s="11"/>
+      <c r="B55" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>45</v>
-      </c>
+      <c r="A56" s="11"/>
       <c r="B56" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+      <c r="A57" s="11"/>
       <c r="B57" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-      <c r="B58" s="2" t="s">
-        <v>48</v>
+      <c r="A58" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="2" t="s">
-        <v>49</v>
+      <c r="A59" s="11"/>
+      <c r="B59" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="A60" s="11" t="s">
         <v>50</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -2138,380 +2105,263 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="3" t="s">
+      <c r="A61" s="11"/>
+      <c r="B61" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="A62" s="11"/>
+      <c r="B62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B62" s="3" t="s">
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="11"/>
+      <c r="B65" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="11"/>
+      <c r="B66" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="11"/>
+      <c r="B68" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="11"/>
+      <c r="B69" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="2" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="2" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="11"/>
+      <c r="B74" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="11"/>
+      <c r="B75" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="11"/>
+      <c r="B76" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="11"/>
+      <c r="B79" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+      <c r="B81" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="4"/>
-      <c r="B68" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="4"/>
-      <c r="B71" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="4"/>
-      <c r="B73" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="4"/>
-      <c r="B74" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="4"/>
-      <c r="B76" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-      <c r="B81" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>63</v>
-      </c>
+      <c r="A82" s="11"/>
       <c r="B82" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4"/>
-      <c r="B83" s="2" t="s">
+      <c r="A83" s="11"/>
+      <c r="B83" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="4"/>
+      <c r="A84" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="B84" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>66</v>
-      </c>
+      <c r="A85" s="11"/>
       <c r="B85" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="4"/>
-      <c r="B86" s="2" t="s">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="11" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4"/>
       <c r="B87" s="2" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
+      <c r="A88" s="11"/>
+      <c r="B88" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B89" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+      <c r="B92" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4"/>
-      <c r="B89" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="4"/>
-      <c r="B90" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B91" s="2" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+      <c r="B94" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="11"/>
+      <c r="B95" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="11"/>
+      <c r="B96" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4"/>
-      <c r="B93" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B95" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="4"/>
-      <c r="B96" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>4</v>
+      <c r="A97" s="11"/>
+      <c r="B97" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="4"/>
-      <c r="B98" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
-      <c r="B107" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
-      <c r="B109" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="4"/>
-      <c r="B111" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="4"/>
-      <c r="B112" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="4"/>
-      <c r="B113" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="4"/>
-      <c r="B114" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="4"/>
-      <c r="B115" s="3" t="s">
-        <v>68</v>
+      <c r="A98" s="11"/>
+      <c r="B98" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="31">
     <mergeCell ref="A19:A21"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A54:A55"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="A28:A30"/>
@@ -2523,26 +2373,20 @@
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A49:A51"/>
     <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="A72:A74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="A88:A90"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="A110:A115"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A99"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A106:A107"/>
+    <mergeCell ref="A80:A83"/>
+    <mergeCell ref="A54:A57"/>
+    <mergeCell ref="A58:A59"/>
+    <mergeCell ref="A60:A63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A93:A98"/>
+    <mergeCell ref="A84:A86"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="A89:A90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
solving ars id mapping file
</commit_message>
<xml_diff>
--- a/data/info_intersecciones.xlsx
+++ b/data/info_intersecciones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="146">
   <si>
     <t>Intersección</t>
   </si>
@@ -220,42 +220,9 @@
     <t>cll44_cr68a</t>
   </si>
   <si>
-    <t>XC-2-ENT-NOR-SUR</t>
-  </si>
-  <si>
-    <t>XC-1-ENT-NOR-SUR</t>
-  </si>
-  <si>
     <t>Entrada</t>
   </si>
   <si>
-    <t>XC-3-ENT-SUR-NOR</t>
-  </si>
-  <si>
-    <t>XC-2-ENT-SUR-NOR</t>
-  </si>
-  <si>
-    <t>XC-1-ENT-SUR-NOR</t>
-  </si>
-  <si>
-    <t>XC-3-ENT-OCC-ORI</t>
-  </si>
-  <si>
-    <t>XC-2-ENT-OCC-ORI</t>
-  </si>
-  <si>
-    <t>XC-1-ENT-OCC-ORI</t>
-  </si>
-  <si>
-    <t>XC-3-ENT-ORI-OCC</t>
-  </si>
-  <si>
-    <t>XC-2-ENT-ORI-OCC</t>
-  </si>
-  <si>
-    <t>XC-1-ENT-ORI-OCC</t>
-  </si>
-  <si>
     <t>XC-2-BOL-65-SAL:OCC-ORI</t>
   </si>
   <si>
@@ -434,6 +401,63 @@
   </si>
   <si>
     <t>Tipo</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-35-ENT:ORI-OCC</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-35-ENT:ORI-OCC</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-35-ENT:SUR-NOR</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-35-ENT:NOR-SUR</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-35-ENT:NOR-SUR</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-33-ENT:OCC-ORI</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-33-ENT:OCC-ORI</t>
+  </si>
+  <si>
+    <t>XC-3-AV80-33-ENT:OCC-ORI</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-33-ENT:ORI-OCC</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-33-ENT:ORI-OCC</t>
+  </si>
+  <si>
+    <t>XC-3-AV80-33-ENT:ORI-OCC</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-33-ENT:NOR-SUR</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-33-ENT:NOR-SUR</t>
+  </si>
+  <si>
+    <t>XC-3-AV80-35-ENT:SUR-NOR</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-35-ENT:OCC-ORI</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-35-ENT:OCC-ORI</t>
+  </si>
+  <si>
+    <t>XC-1-AV80-33-ENT:SUR-NOR</t>
+  </si>
+  <si>
+    <t>XC-2-AV80-33-ENT:SUR-NOR</t>
+  </si>
+  <si>
+    <t>XC-3-AV80-33-ENT:SUR-NOR</t>
   </si>
 </sst>
 </file>
@@ -551,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -568,28 +592,19 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -603,6 +618,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,750 +930,719 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="12"/>
+      <c r="B61" s="17"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="11"/>
+      <c r="D63" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="11"/>
+      <c r="D64" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="11"/>
+      <c r="D68" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="11"/>
+      <c r="D69" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I70" s="19"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="11"/>
+      <c r="D71" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="17"/>
+      <c r="C72" s="11"/>
+      <c r="D72" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
-      <c r="B10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
-      <c r="B18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" s="9" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="12"/>
+      <c r="B73" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
-      <c r="B26" s="9" t="s">
+      <c r="C73" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="12"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="11"/>
+      <c r="D74" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="12"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="11"/>
+      <c r="D75" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="12"/>
+      <c r="B76" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="5" t="s">
+      <c r="C76" s="7" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="15"/>
-      <c r="B28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="15"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="15"/>
-      <c r="B38" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="15"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="15"/>
-      <c r="B44" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="15"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
-      <c r="B57" s="10"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
-      <c r="B62" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D65" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="15"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="10"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
-      <c r="B70" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D70" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="15"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
-      <c r="B73" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D73" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="10"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="D76" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="8"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="12"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="5" t="s">
-        <v>66</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C9"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A31"/>
-    <mergeCell ref="A50:A66"/>
-    <mergeCell ref="A67:A77"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A32:A49"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B38:B43"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="B73:B75"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C47:C49"/>
     <mergeCell ref="C67:C69"/>
     <mergeCell ref="C70:C72"/>
     <mergeCell ref="C73:C75"/>
@@ -1665,8 +1659,41 @@
     <mergeCell ref="C54:C57"/>
     <mergeCell ref="C65:C66"/>
     <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="A24:A31"/>
+    <mergeCell ref="A50:A66"/>
+    <mergeCell ref="A67:A77"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A32:A49"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="B38:B43"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="C21:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1693,7 +1720,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1701,19 +1728,19 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1721,25 +1748,25 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1747,25 +1774,25 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1773,19 +1800,19 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1793,19 +1820,19 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1813,19 +1840,19 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="15"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1833,19 +1860,19 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="15"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1853,19 +1880,19 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="15"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1873,19 +1900,19 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="15"/>
+      <c r="A29" s="12"/>
       <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="12" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1893,25 +1920,25 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1919,19 +1946,19 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="12" t="s">
         <v>34</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1939,25 +1966,25 @@
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="15"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="15"/>
+      <c r="A40" s="12"/>
       <c r="B40" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="15"/>
+      <c r="A41" s="12"/>
       <c r="B41" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1965,13 +1992,13 @@
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="15"/>
+      <c r="A43" s="12"/>
       <c r="B43" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="12" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -1979,19 +2006,19 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="15"/>
+      <c r="A45" s="12"/>
       <c r="B45" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="15"/>
+      <c r="A46" s="12"/>
       <c r="B46" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="12" t="s">
         <v>40</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1999,19 +2026,19 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="15"/>
+      <c r="A48" s="12"/>
       <c r="B48" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="15"/>
+      <c r="A49" s="12"/>
       <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2019,13 +2046,13 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="12"/>
       <c r="B51" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="12" t="s">
         <v>43</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2033,25 +2060,25 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="12"/>
       <c r="B53" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="12"/>
       <c r="B54" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+      <c r="A55" s="12"/>
       <c r="B55" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="12" t="s">
         <v>48</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -2059,13 +2086,13 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+      <c r="A57" s="12"/>
       <c r="B57" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -2073,25 +2100,25 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="12"/>
       <c r="B59" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="12"/>
       <c r="B60" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+      <c r="A61" s="12"/>
       <c r="B61" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="12" t="s">
         <v>51</v>
       </c>
       <c r="B62" s="2" t="s">
@@ -2099,19 +2126,19 @@
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="15"/>
+      <c r="A63" s="12"/>
       <c r="B63" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+      <c r="A64" s="12"/>
       <c r="B64" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -2119,19 +2146,19 @@
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="15"/>
+      <c r="A67" s="12"/>
       <c r="B67" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -2139,19 +2166,19 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
+      <c r="A69" s="12"/>
       <c r="B69" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+      <c r="A70" s="12"/>
       <c r="B70" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -2159,25 +2186,25 @@
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="15"/>
+      <c r="A72" s="12"/>
       <c r="B72" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="15"/>
+      <c r="A73" s="12"/>
       <c r="B73" s="3" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
+      <c r="A74" s="12"/>
       <c r="B74" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
+      <c r="A75" s="12" t="s">
         <v>59</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2185,19 +2212,19 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
+      <c r="A76" s="12"/>
       <c r="B76" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
+      <c r="A77" s="12"/>
       <c r="B77" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="15" t="s">
+      <c r="A78" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -2205,25 +2232,25 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="15"/>
+      <c r="A79" s="12"/>
       <c r="B79" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="15"/>
+      <c r="A80" s="12"/>
       <c r="B80" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="15"/>
+      <c r="A81" s="12"/>
       <c r="B81" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="12" t="s">
         <v>63</v>
       </c>
       <c r="B82" s="2" t="s">
@@ -2231,19 +2258,19 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="15"/>
+      <c r="A83" s="12"/>
       <c r="B83" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="15"/>
+      <c r="A84" s="12"/>
       <c r="B84" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="12" t="s">
         <v>65</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -2251,13 +2278,24 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="15"/>
+      <c r="A86" s="12"/>
       <c r="B86" s="3" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A37"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A46"/>
@@ -2274,17 +2312,6 @@
     <mergeCell ref="A68:A70"/>
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A75:A77"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>